<commit_message>
add region column to master_filtered.csv
</commit_message>
<xml_diff>
--- a/data/master_filtered.xlsx
+++ b/data/master_filtered.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>country_name</t>
   </si>
@@ -262,6 +262,24 @@
   </si>
   <si>
     <t>LTU</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Latin America</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
 </sst>
 </file>
@@ -638,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,9 +675,10 @@
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="10" max="10" width="22.1640625" customWidth="1"/>
     <col min="11" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,8 +712,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -728,8 +750,11 @@
       <c r="K2" s="1">
         <v>1230859428705</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -763,8 +788,11 @@
       <c r="K3" s="1">
         <v>376967406148</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -798,8 +826,11 @@
       <c r="K4" s="1">
         <v>455106661673</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -833,8 +864,11 @@
       <c r="K5" s="1">
         <v>1552807652015</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -868,8 +902,11 @@
       <c r="K6" s="1">
         <v>240796394225</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -903,8 +940,11 @@
       <c r="K7" s="1">
         <v>185156359571</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -938,8 +978,11 @@
       <c r="K8" s="1">
         <v>3363599907530</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -973,8 +1016,11 @@
       <c r="K9" s="1">
         <v>301307828844</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1008,8 +1054,11 @@
       <c r="K10" s="1">
         <v>2858003087966</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1043,8 +1092,11 @@
       <c r="K11" s="1">
         <v>1192955480686</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1078,8 +1130,11 @@
       <c r="K12" s="1">
         <v>231960207681</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1113,8 +1168,11 @@
       <c r="K13" s="1">
         <v>2418945624441</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1148,8 +1206,11 @@
       <c r="K14" s="1">
         <v>194860187692</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1183,8 +1244,11 @@
       <c r="K15" s="1">
         <v>121715203208</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1218,8 +1282,11 @@
       <c r="K16" s="1">
         <v>283716012908</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1253,8 +1320,11 @@
       <c r="K17" s="1">
         <v>299413132027</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1288,8 +1358,11 @@
       <c r="K18" s="1">
         <v>1821579868524</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1323,8 +1396,11 @@
       <c r="K19" s="1">
         <v>4383076298082</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1358,8 +1434,11 @@
       <c r="K20" s="1">
         <v>1377873196261</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1393,8 +1472,11 @@
       <c r="K21" s="1">
         <v>56802211456</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1428,8 +1510,11 @@
       <c r="K22" s="1">
         <v>27004061442</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1463,8 +1548,11 @@
       <c r="K23" s="1">
         <v>1140724180142</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1498,8 +1586,11 @@
       <c r="K24" s="1">
         <v>750318056806</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1533,8 +1624,11 @@
       <c r="K25" s="1">
         <v>386578443733</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1568,8 +1662,11 @@
       <c r="K26" s="1">
         <v>173416551892</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1603,8 +1700,11 @@
       <c r="K27" s="1">
         <v>477066454437</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1638,8 +1738,11 @@
       <c r="K28" s="1">
         <v>199121686400</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1673,8 +1776,11 @@
       <c r="K29" s="1">
         <v>87267593788</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1708,8 +1814,11 @@
       <c r="K30" s="1">
         <v>42776716631</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1743,8 +1852,11 @@
       <c r="K31" s="1">
         <v>495694356612</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1778,8 +1890,11 @@
       <c r="K32" s="1">
         <v>717887918353</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -1813,8 +1928,11 @@
       <c r="K33" s="1">
         <v>18036648000000</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -1848,8 +1966,11 @@
       <c r="K34" s="1">
         <v>292080160448</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -1883,8 +2004,11 @@
       <c r="K35" s="1">
         <v>52958365929</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1917,6 +2041,9 @@
       </c>
       <c r="K36" s="1">
         <v>41402022148</v>
+      </c>
+      <c r="L36" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change yColumn to percentile
</commit_message>
<xml_diff>
--- a/data/master_filtered.xlsx
+++ b/data/master_filtered.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="8720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
   <si>
     <t>country_name</t>
   </si>
@@ -280,13 +280,16 @@
   </si>
   <si>
     <t>Asia</t>
+  </si>
+  <si>
+    <t>percentile_average_mean_score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -298,6 +301,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,15 +336,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 14 2" xfId="1"/>
   </cellStyles>
@@ -656,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -673,12 +696,12 @@
     <col min="7" max="7" width="23.33203125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="22.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,13 +733,16 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -747,14 +773,18 @@
       <c r="J2">
         <v>502.26355319709529</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2">
+        <f>_xlfn.PERCENTRANK.INC($J$2:$J$36,J2,2) * 100</f>
+        <v>61</v>
+      </c>
+      <c r="L2" s="1">
         <v>1230859428705</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -785,14 +815,18 @@
       <c r="J3">
         <v>492.21513227730537</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3">
+        <f t="shared" ref="K3:K36" si="0">_xlfn.PERCENTRANK.INC($J$2:$J$36,J3,2) * 100</f>
+        <v>47</v>
+      </c>
+      <c r="L3" s="1">
         <v>376967406148</v>
       </c>
-      <c r="L3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -823,14 +857,18 @@
       <c r="J4">
         <v>502.50276322463372</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="L4" s="1">
         <v>455106661673</v>
       </c>
-      <c r="L4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -861,14 +899,18 @@
       <c r="J5">
         <v>523.33996842790395</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="L5" s="1">
         <v>1552807652015</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -899,14 +941,18 @@
       <c r="J6">
         <v>442.73279199563495</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L6" s="1">
         <v>240796394225</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -937,14 +983,18 @@
       <c r="J7">
         <v>490.80184733752321</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="L7" s="1">
         <v>185156359571</v>
       </c>
-      <c r="L7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -975,14 +1025,18 @@
       <c r="J8">
         <v>508.07201281555217</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="L8" s="1">
         <v>3363599907530</v>
       </c>
-      <c r="L8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1013,14 +1067,18 @@
       <c r="J9">
         <v>504.27969501934177</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="L9" s="1">
         <v>301307828844</v>
       </c>
-      <c r="L9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1051,14 +1109,18 @@
       <c r="J10">
         <v>499.89064393192274</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>57.999999999999993</v>
+      </c>
+      <c r="L10" s="1">
         <v>2858003087966</v>
       </c>
-      <c r="L10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1089,14 +1151,18 @@
       <c r="J11">
         <v>491.40191177538958</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="L11" s="1">
         <v>1192955480686</v>
       </c>
-      <c r="L11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1127,14 +1193,18 @@
       <c r="J12">
         <v>522.72094967190299</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="L12" s="1">
         <v>231960207681</v>
       </c>
-      <c r="L12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1165,14 +1235,18 @@
       <c r="J13">
         <v>495.73471370311336</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L13" s="1">
         <v>2418945624441</v>
       </c>
-      <c r="L13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1203,14 +1277,18 @@
       <c r="J14">
         <v>458.4994127528737</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="L14" s="1">
         <v>194860187692</v>
       </c>
-      <c r="L14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1241,14 +1319,18 @@
       <c r="J15">
         <v>474.36721898719105</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="L15" s="1">
         <v>121715203208</v>
       </c>
-      <c r="L15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1279,14 +1361,18 @@
       <c r="J16">
         <v>509.03731371616459</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="L16" s="1">
         <v>283716012908</v>
       </c>
-      <c r="L16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1317,14 +1403,18 @@
       <c r="J17">
         <v>471.72764807570212</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="L17" s="1">
         <v>299413132027</v>
       </c>
-      <c r="L17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1355,14 +1445,18 @@
       <c r="J18">
         <v>485.01116550001575</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L18" s="1">
         <v>1821579868524</v>
       </c>
-      <c r="L18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1393,14 +1487,18 @@
       <c r="J19">
         <v>528.93106000946341</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L19" s="1">
         <v>4383076298082</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1431,14 +1529,18 @@
       <c r="J20">
         <v>519.11760282114358</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="L20" s="1">
         <v>1377873196261</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1469,14 +1571,18 @@
       <c r="J21">
         <v>483.33869454343812</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>28.999999999999996</v>
+      </c>
+      <c r="L21" s="1">
         <v>56802211456</v>
       </c>
-      <c r="L21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1507,14 +1613,18 @@
       <c r="J22">
         <v>486.76273379079004</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="L22" s="1">
         <v>27004061442</v>
       </c>
-      <c r="L22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1545,14 +1655,18 @@
       <c r="J23">
         <v>415.66995992083304</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L23" s="1">
         <v>1140724180142</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1583,14 +1697,18 @@
       <c r="J24">
         <v>507.92888366554189</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="L24" s="1">
         <v>750318056806</v>
       </c>
-      <c r="L24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1621,14 +1739,18 @@
       <c r="J25">
         <v>504.46735746946496</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="L25" s="1">
         <v>386578443733</v>
       </c>
-      <c r="L25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1659,14 +1781,18 @@
       <c r="J26">
         <v>505.93250400734217</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="L26" s="1">
         <v>173416551892</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1697,14 +1823,18 @@
       <c r="J27">
         <v>503.86722350729883</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="L27" s="1">
         <v>477066454437</v>
       </c>
-      <c r="L27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1735,14 +1865,18 @@
       <c r="J28">
         <v>496.95200153992988</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="L28" s="1">
         <v>199121686400</v>
       </c>
-      <c r="L28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1773,14 +1907,18 @@
       <c r="J29">
         <v>462.83977921673187</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="L29" s="1">
         <v>87267593788</v>
       </c>
-      <c r="L29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1811,14 +1949,18 @@
       <c r="J30">
         <v>509.33302716544137</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="L30" s="1">
         <v>42776716631</v>
       </c>
-      <c r="L30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1849,14 +1991,18 @@
       <c r="J31">
         <v>495.83203565177263</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="L31" s="1">
         <v>495694356612</v>
       </c>
-      <c r="L31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1887,14 +2033,18 @@
       <c r="J32">
         <v>424.75953115150941</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L32" s="1">
         <v>717887918353</v>
       </c>
-      <c r="L32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -1925,14 +2075,18 @@
       <c r="J33">
         <v>487.60199904942937</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="L33" s="1">
         <v>18036648000000</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -1963,14 +2117,18 @@
       <c r="J34">
         <v>410.09258900630812</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
         <v>292080160448</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2001,14 +2159,18 @@
       <c r="J35">
         <v>415.78298207496772</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L35" s="1">
         <v>52958365929</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2039,15 +2201,20 @@
       <c r="J36">
         <v>475.3996180374898</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="L36" s="1">
         <v>41402022148</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add percentile rank column to all test score columns
</commit_message>
<xml_diff>
--- a/data/master_filtered.xlsx
+++ b/data/master_filtered.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="8720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>country_name</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>percentile_average_mean_score</t>
+  </si>
+  <si>
+    <t>percentile_reading_mean_score</t>
+  </si>
+  <si>
+    <t>percentile_math_mean_score</t>
+  </si>
+  <si>
+    <t>percentile_science_mean_score</t>
   </si>
 </sst>
 </file>
@@ -679,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -693,15 +702,15 @@
     <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="11" width="22.1640625" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="10" width="20" customWidth="1"/>
+    <col min="11" max="12" width="23" customWidth="1"/>
+    <col min="13" max="14" width="22.1640625" customWidth="1"/>
+    <col min="15" max="15" width="20.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -724,25 +733,34 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>87</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -765,26 +783,38 @@
         <v>509.9939</v>
       </c>
       <c r="H2">
+        <f>_xlfn.PERCENTRANK.INC($G$2:$G$36,G2,2) * 100</f>
+        <v>82</v>
+      </c>
+      <c r="I2">
         <v>493.89620000000002</v>
       </c>
-      <c r="I2">
+      <c r="J2">
+        <f>_xlfn.PERCENTRANK.INC($I$2:$I$36,I2,2) * 100</f>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="K2">
         <v>502.9005595912858</v>
       </c>
-      <c r="J2">
+      <c r="L2">
+        <f>_xlfn.PERCENTRANK.INC($K$2:$K$36,K2,2) * 100</f>
+        <v>67</v>
+      </c>
+      <c r="M2">
         <v>502.26355319709529</v>
       </c>
-      <c r="K2">
-        <f>_xlfn.PERCENTRANK.INC($J$2:$J$36,J2,2) * 100</f>
+      <c r="N2">
+        <f>_xlfn.PERCENTRANK.INC($M$2:$M$36,M2,2) * 100</f>
         <v>61</v>
       </c>
-      <c r="L2" s="1">
+      <c r="O2" s="1">
         <v>1230859428705</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -807,26 +837,38 @@
         <v>495.03750000000002</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H36" si="0">_xlfn.PERCENTRANK.INC($G$2:$G$36,G3,2) * 100</f>
+        <v>50</v>
+      </c>
+      <c r="I3">
         <v>496.7423</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <f t="shared" ref="J3:J36" si="1">_xlfn.PERCENTRANK.INC($I$2:$I$36,I3,2) * 100</f>
+        <v>64</v>
+      </c>
+      <c r="K3">
         <v>484.86559683191604</v>
       </c>
-      <c r="J3">
+      <c r="L3">
+        <f t="shared" ref="L3:L36" si="2">_xlfn.PERCENTRANK.INC($K$2:$K$36,K3,2) * 100</f>
+        <v>35</v>
+      </c>
+      <c r="M3">
         <v>492.21513227730537</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K36" si="0">_xlfn.PERCENTRANK.INC($J$2:$J$36,J3,2) * 100</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N36" si="3">_xlfn.PERCENTRANK.INC($M$2:$M$36,M3,2) * 100</f>
         <v>47</v>
       </c>
-      <c r="L3" s="1">
+      <c r="O3" s="1">
         <v>376967406148</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -849,26 +891,38 @@
         <v>501.99970000000002</v>
       </c>
       <c r="H4">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="I4">
         <v>506.98439999999999</v>
       </c>
-      <c r="I4">
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="K4">
         <v>498.52418967390116</v>
       </c>
-      <c r="J4">
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="M4">
         <v>502.50276322463372</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
+      <c r="N4">
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="L4" s="1">
+      <c r="O4" s="1">
         <v>455106661673</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -891,26 +945,38 @@
         <v>527.7047</v>
       </c>
       <c r="H5">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="I5">
         <v>515.64739999999995</v>
       </c>
-      <c r="I5">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="K5">
         <v>526.6678052837118</v>
       </c>
-      <c r="J5">
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="M5">
         <v>523.33996842790395</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
+      <c r="N5">
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="L5" s="1">
+      <c r="O5" s="1">
         <v>1552807652015</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -933,26 +999,38 @@
         <v>446.95609999999999</v>
       </c>
       <c r="H6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I6">
         <v>422.67140000000001</v>
       </c>
-      <c r="I6">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="K6">
         <v>458.57087598690481</v>
       </c>
-      <c r="J6">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="M6">
         <v>442.73279199563495</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
+      <c r="N6">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="L6" s="1">
+      <c r="O6" s="1">
         <v>240796394225</v>
       </c>
-      <c r="M6" t="s">
+      <c r="P6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -975,26 +1053,38 @@
         <v>492.83</v>
       </c>
       <c r="H7">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="I7">
         <v>492.3254</v>
       </c>
-      <c r="I7">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="K7">
         <v>487.25014201256977</v>
       </c>
-      <c r="J7">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="M7">
         <v>490.80184733752321</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
+      <c r="N7">
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="L7" s="1">
+      <c r="O7" s="1">
         <v>185156359571</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1017,26 +1107,38 @@
         <v>509.14060000000001</v>
       </c>
       <c r="H8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="I8">
         <v>505.97129999999999</v>
       </c>
-      <c r="I8">
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="K8">
         <v>509.10413844665646</v>
       </c>
-      <c r="J8">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="M8">
         <v>508.07201281555217</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
+      <c r="N8">
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="L8" s="1">
+      <c r="O8" s="1">
         <v>3363599907530</v>
       </c>
-      <c r="M8" t="s">
+      <c r="P8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1059,26 +1161,38 @@
         <v>501.93689999999998</v>
       </c>
       <c r="H9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="I9">
         <v>511.08760000000001</v>
       </c>
-      <c r="I9">
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="K9">
         <v>499.81458505802533</v>
       </c>
-      <c r="J9">
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="M9">
         <v>504.27969501934177</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
+      <c r="N9">
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="L9" s="1">
+      <c r="O9" s="1">
         <v>301307828844</v>
       </c>
-      <c r="M9" t="s">
+      <c r="P9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1101,26 +1215,38 @@
         <v>509.22149999999999</v>
       </c>
       <c r="H10">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="I10">
         <v>492.4785</v>
       </c>
-      <c r="I10">
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K10">
         <v>497.97193179576811</v>
       </c>
-      <c r="J10">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="M10">
         <v>499.89064393192274</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
+      <c r="N10">
+        <f t="shared" si="3"/>
         <v>57.999999999999993</v>
       </c>
-      <c r="L10" s="1">
+      <c r="O10" s="1">
         <v>2858003087966</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1143,26 +1269,38 @@
         <v>492.78609999999998</v>
       </c>
       <c r="H11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="I11">
         <v>485.84320000000002</v>
       </c>
-      <c r="I11">
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="K11">
         <v>495.57643532616868</v>
       </c>
-      <c r="J11">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="M11">
         <v>491.40191177538958</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
+      <c r="N11">
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="L11" s="1">
+      <c r="O11" s="1">
         <v>1192955480686</v>
       </c>
-      <c r="M11" t="s">
+      <c r="P11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1185,26 +1323,38 @@
         <v>530.66120000000001</v>
       </c>
       <c r="H12">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="I12">
         <v>511.07690000000002</v>
       </c>
-      <c r="I12">
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="K12">
         <v>526.42474901570904</v>
       </c>
-      <c r="J12">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="M12">
         <v>522.72094967190299</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
+      <c r="N12">
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="L12" s="1">
+      <c r="O12" s="1">
         <v>231960207681</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1227,26 +1377,38 @@
         <v>494.9776</v>
       </c>
       <c r="H13">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="I13">
         <v>492.92039999999997</v>
       </c>
-      <c r="I13">
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="K13">
         <v>499.30614110934005</v>
       </c>
-      <c r="J13">
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>57.999999999999993</v>
+      </c>
+      <c r="M13">
         <v>495.73471370311336</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
+      <c r="N13">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="L13" s="1">
+      <c r="O13" s="1">
         <v>2418945624441</v>
       </c>
-      <c r="M13" t="s">
+      <c r="P13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1269,26 +1431,38 @@
         <v>454.8288</v>
       </c>
       <c r="H14">
+        <f t="shared" si="0"/>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="I14">
         <v>453.62990000000002</v>
       </c>
-      <c r="I14">
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="K14">
         <v>467.03953825862101</v>
       </c>
-      <c r="J14">
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="M14">
         <v>458.4994127528737</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
+      <c r="N14">
+        <f t="shared" si="3"/>
         <v>14.000000000000002</v>
       </c>
-      <c r="L14" s="1">
+      <c r="O14" s="1">
         <v>194860187692</v>
       </c>
-      <c r="M14" t="s">
+      <c r="P14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1311,26 +1485,38 @@
         <v>476.7475</v>
       </c>
       <c r="H15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I15">
         <v>476.83089999999999</v>
       </c>
-      <c r="I15">
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="K15">
         <v>469.52325696157317</v>
       </c>
-      <c r="J15">
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M15">
         <v>474.36721898719105</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
+      <c r="N15">
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="L15" s="1">
+      <c r="O15" s="1">
         <v>121715203208</v>
       </c>
-      <c r="M15" t="s">
+      <c r="P15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1353,26 +1539,38 @@
         <v>502.57510000000002</v>
       </c>
       <c r="H16">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="I16">
         <v>503.72199999999998</v>
       </c>
-      <c r="I16">
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="K16">
         <v>520.81484114849388</v>
       </c>
-      <c r="J16">
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="M16">
         <v>509.03731371616459</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
+      <c r="N16">
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="L16" s="1">
+      <c r="O16" s="1">
         <v>283716012908</v>
       </c>
-      <c r="M16" t="s">
+      <c r="P16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1395,26 +1593,38 @@
         <v>466.55279999999999</v>
       </c>
       <c r="H17">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I17">
         <v>469.66950000000003</v>
       </c>
-      <c r="I17">
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K17">
         <v>478.96064422710646</v>
       </c>
-      <c r="J17">
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="M17">
         <v>471.72764807570212</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
+      <c r="N17">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="L17" s="1">
+      <c r="O17" s="1">
         <v>299413132027</v>
       </c>
-      <c r="M17" t="s">
+      <c r="P17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1437,26 +1647,38 @@
         <v>480.54680000000002</v>
       </c>
       <c r="H18">
+        <f t="shared" si="0"/>
+        <v>28.999999999999996</v>
+      </c>
+      <c r="I18">
         <v>489.7287</v>
       </c>
-      <c r="I18">
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="K18">
         <v>484.75799650004728</v>
       </c>
-      <c r="J18">
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="M18">
         <v>485.01116550001575</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
+      <c r="N18">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="L18" s="1">
+      <c r="O18" s="1">
         <v>1821579868524</v>
       </c>
-      <c r="M18" t="s">
+      <c r="P18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1479,26 +1701,38 @@
         <v>538.39480000000003</v>
       </c>
       <c r="H19">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I19">
         <v>532.43989999999997</v>
       </c>
-      <c r="I19">
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="K19">
         <v>515.95848002839034</v>
       </c>
-      <c r="J19">
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="M19">
         <v>528.93106000946341</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
+      <c r="N19">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="L19" s="1">
+      <c r="O19" s="1">
         <v>4383076298082</v>
       </c>
-      <c r="M19" t="s">
+      <c r="P19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1521,26 +1755,38 @@
         <v>515.80989999999997</v>
       </c>
       <c r="H20">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="I20">
         <v>524.10619999999994</v>
       </c>
-      <c r="I20">
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="K20">
         <v>517.43670846343105</v>
       </c>
-      <c r="J20">
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="M20">
         <v>519.11760282114358</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
+      <c r="N20">
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
-      <c r="L20" s="1">
+      <c r="O20" s="1">
         <v>1377873196261</v>
       </c>
-      <c r="M20" t="s">
+      <c r="P20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1563,26 +1809,38 @@
         <v>482.8064</v>
       </c>
       <c r="H21">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I21">
         <v>485.7706</v>
       </c>
-      <c r="I21">
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="K21">
         <v>481.43908363031443</v>
       </c>
-      <c r="J21">
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>28.999999999999996</v>
+      </c>
+      <c r="M21">
         <v>483.33869454343812</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
+      <c r="N21">
+        <f t="shared" si="3"/>
         <v>28.999999999999996</v>
       </c>
-      <c r="L21" s="1">
+      <c r="O21" s="1">
         <v>56802211456</v>
       </c>
-      <c r="M21" t="s">
+      <c r="P21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1605,26 +1863,38 @@
         <v>490.22500000000002</v>
       </c>
       <c r="H22">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="I22">
         <v>482.30509999999998</v>
       </c>
-      <c r="I22">
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K22">
         <v>487.75810137237016</v>
       </c>
-      <c r="J22">
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="M22">
         <v>486.76273379079004</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
+      <c r="N22">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="L22" s="1">
+      <c r="O22" s="1">
         <v>27004061442</v>
       </c>
-      <c r="M22" t="s">
+      <c r="P22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1647,26 +1917,38 @@
         <v>415.7099</v>
       </c>
       <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>408.02350000000001</v>
       </c>
-      <c r="I23">
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K23">
         <v>423.27647976249904</v>
       </c>
-      <c r="J23">
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M23">
         <v>415.66995992083304</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
+      <c r="N23">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L23" s="1">
+      <c r="O23" s="1">
         <v>1140724180142</v>
       </c>
-      <c r="M23" t="s">
+      <c r="P23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1689,26 +1971,38 @@
         <v>508.57479999999998</v>
       </c>
       <c r="H24">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="I24">
         <v>512.25279999999998</v>
       </c>
-      <c r="I24">
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="K24">
         <v>502.95905099662582</v>
       </c>
-      <c r="J24">
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="M24">
         <v>507.92888366554189</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
+      <c r="N24">
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="L24" s="1">
+      <c r="O24" s="1">
         <v>750318056806</v>
       </c>
-      <c r="M24" t="s">
+      <c r="P24" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1731,26 +2025,38 @@
         <v>498.48110000000003</v>
       </c>
       <c r="H25">
+        <f t="shared" si="0"/>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="I25">
         <v>501.72980000000001</v>
       </c>
-      <c r="I25">
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="K25">
         <v>513.19117240839489</v>
       </c>
-      <c r="J25">
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="M25">
         <v>504.46735746946496</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
+      <c r="N25">
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="L25" s="1">
+      <c r="O25" s="1">
         <v>386578443733</v>
       </c>
-      <c r="M25" t="s">
+      <c r="P25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1773,26 +2079,38 @@
         <v>513.30349999999999</v>
       </c>
       <c r="H26">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="I26">
         <v>495.22329999999999</v>
       </c>
-      <c r="I26">
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="K26">
         <v>509.27071202202643</v>
       </c>
-      <c r="J26">
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="M26">
         <v>505.93250400734217</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
+      <c r="N26">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="L26" s="1">
+      <c r="O26" s="1">
         <v>173416551892</v>
       </c>
-      <c r="M26" t="s">
+      <c r="P26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1815,26 +2133,38 @@
         <v>501.43529999999998</v>
       </c>
       <c r="H27">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="I27">
         <v>504.46929999999998</v>
       </c>
-      <c r="I27">
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="K27">
         <v>505.69707052189653</v>
       </c>
-      <c r="J27">
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="M27">
         <v>503.86722350729883</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
+      <c r="N27">
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="L27" s="1">
+      <c r="O27" s="1">
         <v>477066454437</v>
       </c>
-      <c r="M27" t="s">
+      <c r="P27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1857,26 +2187,38 @@
         <v>501.1001</v>
       </c>
       <c r="H28">
+        <f t="shared" si="0"/>
+        <v>57.999999999999993</v>
+      </c>
+      <c r="I28">
         <v>491.62700000000001</v>
       </c>
-      <c r="I28">
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="K28">
         <v>498.12890461978964</v>
       </c>
-      <c r="J28">
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="M28">
         <v>496.95200153992988</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
+      <c r="N28">
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="L28" s="1">
+      <c r="O28" s="1">
         <v>199121686400</v>
       </c>
-      <c r="M28" t="s">
+      <c r="P28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1899,26 +2241,38 @@
         <v>460.7749</v>
       </c>
       <c r="H29">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="I29">
         <v>475.23009999999999</v>
       </c>
-      <c r="I29">
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="K29">
         <v>452.51433765019578</v>
       </c>
-      <c r="J29">
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="M29">
         <v>462.83977921673187</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
+      <c r="N29">
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="L29" s="1">
+      <c r="O29" s="1">
         <v>87267593788</v>
       </c>
-      <c r="M29" t="s">
+      <c r="P29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1941,26 +2295,38 @@
         <v>512.86360000000002</v>
       </c>
       <c r="H30">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="I30">
         <v>509.9196</v>
       </c>
-      <c r="I30">
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="K30">
         <v>505.21588149632402</v>
       </c>
-      <c r="J30">
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="M30">
         <v>509.33302716544137</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
+      <c r="N30">
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="L30" s="1">
+      <c r="O30" s="1">
         <v>42776716631</v>
       </c>
-      <c r="M30" t="s">
+      <c r="P30" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1983,26 +2349,38 @@
         <v>493.42239999999998</v>
       </c>
       <c r="H31">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="I31">
         <v>493.91809999999998</v>
       </c>
-      <c r="I31">
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>57.999999999999993</v>
+      </c>
+      <c r="K31">
         <v>500.15560695531786</v>
       </c>
-      <c r="J31">
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="M31">
         <v>495.83203565177263</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
+      <c r="N31">
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="L31" s="1">
+      <c r="O31" s="1">
         <v>495694356612</v>
       </c>
-      <c r="M31" t="s">
+      <c r="P31" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2025,26 +2403,38 @@
         <v>425.48950000000002</v>
       </c>
       <c r="H32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I32">
         <v>420.45400000000001</v>
       </c>
-      <c r="I32">
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K32">
         <v>428.33509345452796</v>
       </c>
-      <c r="J32">
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M32">
         <v>424.75953115150941</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="0"/>
+      <c r="N32">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L32" s="1">
+      <c r="O32" s="1">
         <v>717887918353</v>
       </c>
-      <c r="M32" t="s">
+      <c r="P32" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2067,26 +2457,38 @@
         <v>496.24239999999998</v>
       </c>
       <c r="H33">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="I33">
         <v>469.62849999999997</v>
       </c>
-      <c r="I33">
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="K33">
         <v>496.93509714828809</v>
       </c>
-      <c r="J33">
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="M33">
         <v>487.60199904942937</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="0"/>
+      <c r="N33">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="L33" s="1">
+      <c r="O33" s="1">
         <v>18036648000000</v>
       </c>
-      <c r="M33" t="s">
+      <c r="P33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2109,26 +2511,38 @@
         <v>415.72879999999998</v>
       </c>
       <c r="H34">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I34">
         <v>389.6438</v>
       </c>
-      <c r="I34">
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K34">
         <v>424.90516701892449</v>
       </c>
-      <c r="J34">
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M34">
         <v>410.09258900630812</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="0"/>
+      <c r="N34">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L34" s="1">
+      <c r="O34" s="1">
         <v>292080160448</v>
       </c>
-      <c r="M34" t="s">
+      <c r="P34" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2151,26 +2565,38 @@
         <v>419.608</v>
       </c>
       <c r="H35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I35">
         <v>400.2534</v>
       </c>
-      <c r="I35">
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K35">
         <v>427.48754622490299</v>
       </c>
-      <c r="J35">
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M35">
         <v>415.78298207496772</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="0"/>
+      <c r="N35">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="L35" s="1">
+      <c r="O35" s="1">
         <v>52958365929</v>
       </c>
-      <c r="M35" t="s">
+      <c r="P35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2193,22 +2619,34 @@
         <v>475.40890000000002</v>
       </c>
       <c r="H36">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="I36">
         <v>478.38339999999999</v>
       </c>
-      <c r="I36">
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>28.999999999999996</v>
+      </c>
+      <c r="K36">
         <v>472.40655411246945</v>
       </c>
-      <c r="J36">
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="M36">
         <v>475.3996180374898</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="0"/>
+      <c r="N36">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="L36" s="1">
+      <c r="O36" s="1">
         <v>41402022148</v>
       </c>
-      <c r="M36" t="s">
+      <c r="P36" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>